<commit_message>
Update data and formatting code
</commit_message>
<xml_diff>
--- a/DataFormat/EditedData/Data_UDZ_harveyi_spadix_Nov18.xlsx
+++ b/DataFormat/EditedData/Data_UDZ_harveyi_spadix_Nov18.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farrm\Documents\GitHub\HMSNO\DataFormat\EditedData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farrmt\Documents\HMSNO\DataFormat\EditedData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608A2F12-E39E-4B98-864E-B869BE80EA64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19740" windowHeight="8805"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="harveyi" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="84">
   <si>
     <t>CT-UDZ-1-01</t>
   </si>
@@ -275,11 +276,14 @@
   <si>
     <t>density</t>
   </si>
+  <si>
+    <t>MTF edited on Aug 10 2020: missing row</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -300,7 +304,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -311,6 +315,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -335,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
@@ -361,6 +371,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,10 +655,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW541"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A503" workbookViewId="0">
+    <sheetView topLeftCell="A383" workbookViewId="0">
       <selection activeCell="Y537" sqref="Y537"/>
     </sheetView>
   </sheetViews>
@@ -34287,11 +34302,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ540"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AQ541"/>
   <sheetViews>
-    <sheetView topLeftCell="A503" workbookViewId="0">
-      <selection activeCell="X538" sqref="X538"/>
+    <sheetView tabSelected="1" topLeftCell="A420" workbookViewId="0">
+      <selection activeCell="AG445" sqref="AG445"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -61109,7 +61124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="433" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A433" s="10" t="s">
         <v>11</v>
       </c>
@@ -61171,7 +61186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="434" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A434" s="10" t="s">
         <v>12</v>
       </c>
@@ -61233,7 +61248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="435" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A435" s="10" t="s">
         <v>13</v>
       </c>
@@ -61295,7 +61310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="436" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A436" s="10" t="s">
         <v>14</v>
       </c>
@@ -61357,7 +61372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="437" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A437" s="10" t="s">
         <v>15</v>
       </c>
@@ -61419,7 +61434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="438" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A438" s="10" t="s">
         <v>16</v>
       </c>
@@ -61481,71 +61496,75 @@
         <v>0</v>
       </c>
     </row>
-    <row r="439" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A439" s="10" t="s">
+    <row r="439" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A439" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B439" s="16">
+        <v>0</v>
+      </c>
+      <c r="C439" s="16">
+        <v>0</v>
+      </c>
+      <c r="D439" s="16">
+        <v>0</v>
+      </c>
+      <c r="E439" s="16">
+        <v>0</v>
+      </c>
+      <c r="F439" s="16">
+        <v>0</v>
+      </c>
+      <c r="G439" s="16">
+        <v>0</v>
+      </c>
+      <c r="H439" s="17"/>
+      <c r="I439" s="17">
+        <v>2016</v>
+      </c>
+      <c r="J439" s="17">
+        <v>0</v>
+      </c>
+      <c r="K439" s="17">
+        <v>0</v>
+      </c>
+      <c r="L439" s="17">
+        <v>0</v>
+      </c>
+      <c r="M439" s="17">
+        <v>0</v>
+      </c>
+      <c r="N439" s="17">
+        <v>0</v>
+      </c>
+      <c r="O439" s="17">
+        <v>0</v>
+      </c>
+      <c r="P439" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q439" s="17">
+        <v>0</v>
+      </c>
+      <c r="R439" s="17">
+        <v>0</v>
+      </c>
+      <c r="S439" s="17">
+        <v>-0.50467062641897742</v>
+      </c>
+      <c r="T439" s="17">
+        <v>-0.46626233467977302</v>
+      </c>
+      <c r="U439" s="17">
+        <v>0</v>
+      </c>
+      <c r="V439" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="440" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A440" s="10" t="s">
         <v>18</v>
-      </c>
-      <c r="B439" s="6">
-        <v>0</v>
-      </c>
-      <c r="C439" s="6">
-        <v>0</v>
-      </c>
-      <c r="D439" s="6">
-        <v>0</v>
-      </c>
-      <c r="E439" s="6">
-        <v>0</v>
-      </c>
-      <c r="F439" s="6">
-        <v>0</v>
-      </c>
-      <c r="G439" s="6">
-        <v>0</v>
-      </c>
-      <c r="I439" s="9">
-        <v>2016</v>
-      </c>
-      <c r="J439">
-        <v>0</v>
-      </c>
-      <c r="K439">
-        <v>0</v>
-      </c>
-      <c r="L439">
-        <v>0</v>
-      </c>
-      <c r="M439">
-        <v>0</v>
-      </c>
-      <c r="N439">
-        <v>0</v>
-      </c>
-      <c r="O439">
-        <v>0</v>
-      </c>
-      <c r="P439">
-        <v>0</v>
-      </c>
-      <c r="Q439">
-        <v>1</v>
-      </c>
-      <c r="R439">
-        <v>0</v>
-      </c>
-      <c r="S439">
-        <v>-0.50467062641897742</v>
-      </c>
-      <c r="T439">
-        <v>-0.46626233467977302</v>
-      </c>
-      <c r="U439">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="440" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A440" s="10" t="s">
-        <v>19</v>
       </c>
       <c r="B440" s="6">
         <v>0</v>
@@ -61596,18 +61615,18 @@
         <v>0</v>
       </c>
       <c r="S440">
-        <v>-1.5705178501640182</v>
+        <v>-0.50467062641897742</v>
       </c>
       <c r="T440">
-        <v>-0.62701770326260997</v>
+        <v>-0.46626233467977302</v>
       </c>
       <c r="U440">
         <v>0</v>
       </c>
     </row>
-    <row r="441" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A441" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B441" s="6">
         <v>0</v>
@@ -61616,10 +61635,10 @@
         <v>0</v>
       </c>
       <c r="D441" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E441" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F441" s="6">
         <v>0</v>
@@ -61658,36 +61677,36 @@
         <v>0</v>
       </c>
       <c r="S441">
-        <v>-1.6535361012597376</v>
+        <v>-1.5705178501640182</v>
       </c>
       <c r="T441">
-        <v>-0.86240949297319258</v>
+        <v>-0.62701770326260997</v>
       </c>
       <c r="U441">
         <v>0</v>
       </c>
     </row>
-    <row r="442" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A442" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B442" s="6">
         <v>0</v>
       </c>
       <c r="C442" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D442" s="6">
         <v>1</v>
       </c>
       <c r="E442" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F442" s="6">
         <v>0</v>
       </c>
       <c r="G442" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I442" s="9">
         <v>2016</v>
@@ -61720,27 +61739,27 @@
         <v>0</v>
       </c>
       <c r="S442">
-        <v>-0.68409716910972551</v>
+        <v>-1.6535361012597376</v>
       </c>
       <c r="T442">
-        <v>-0.88250391404604722</v>
+        <v>-0.86240949297319258</v>
       </c>
       <c r="U442">
         <v>0</v>
       </c>
     </row>
-    <row r="443" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A443" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B443" s="6">
         <v>0</v>
       </c>
       <c r="C443" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D443" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E443" s="6">
         <v>0</v>
@@ -61749,7 +61768,7 @@
         <v>0</v>
       </c>
       <c r="G443" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I443" s="9">
         <v>2016</v>
@@ -61782,18 +61801,18 @@
         <v>0</v>
       </c>
       <c r="S443">
-        <v>-0.68141916100986355</v>
+        <v>-0.68409716910972551</v>
       </c>
       <c r="T443">
-        <v>-0.61266454535342807</v>
+        <v>-0.88250391404604722</v>
       </c>
       <c r="U443">
         <v>0</v>
       </c>
     </row>
-    <row r="444" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A444" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B444" s="6">
         <v>0</v>
@@ -61844,18 +61863,18 @@
         <v>0</v>
       </c>
       <c r="S444">
-        <v>-9.4935387140104896E-2</v>
+        <v>-0.68141916100986355</v>
       </c>
       <c r="T444">
-        <v>3.0356928977919619E-2</v>
+        <v>-0.61266454535342807</v>
       </c>
       <c r="U444">
         <v>0</v>
       </c>
     </row>
-    <row r="445" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A445" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B445" s="6">
         <v>0</v>
@@ -61864,7 +61883,7 @@
         <v>0</v>
       </c>
       <c r="D445" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E445" s="6">
         <v>0</v>
@@ -61906,18 +61925,18 @@
         <v>0</v>
       </c>
       <c r="S445">
-        <v>-1.3455651697756177</v>
+        <v>-9.4935387140104896E-2</v>
       </c>
       <c r="T445">
-        <v>-5.4326702686253406E-2</v>
+        <v>3.0356928977919619E-2</v>
       </c>
       <c r="U445">
         <v>0</v>
       </c>
     </row>
-    <row r="446" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A446" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B446" s="6">
         <v>0</v>
@@ -61926,10 +61945,10 @@
         <v>0</v>
       </c>
       <c r="D446" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E446" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F446" s="6">
         <v>0</v>
@@ -61968,30 +61987,30 @@
         <v>0</v>
       </c>
       <c r="S446">
-        <v>0.95484378800576453</v>
+        <v>-1.3455651697756177</v>
       </c>
       <c r="T446">
-        <v>-0.63275896642628271</v>
+        <v>-5.4326702686253406E-2</v>
       </c>
       <c r="U446">
         <v>0</v>
       </c>
     </row>
-    <row r="447" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A447" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B447" s="6">
         <v>0</v>
       </c>
       <c r="C447" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D447" s="6">
         <v>0</v>
       </c>
       <c r="E447" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F447" s="6">
         <v>0</v>
@@ -62030,27 +62049,27 @@
         <v>0</v>
       </c>
       <c r="S447">
-        <v>0.72989110761736398</v>
+        <v>0.95484378800576453</v>
       </c>
       <c r="T447">
-        <v>-0.67438312436291015</v>
+        <v>-0.63275896642628271</v>
       </c>
       <c r="U447">
         <v>0</v>
       </c>
     </row>
-    <row r="448" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A448" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B448" s="6">
         <v>0</v>
       </c>
       <c r="C448" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D448" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E448" s="6">
         <v>0</v>
@@ -62092,10 +62111,10 @@
         <v>0</v>
       </c>
       <c r="S448">
-        <v>0.85843549641073569</v>
+        <v>0.72989110761736398</v>
       </c>
       <c r="T448">
-        <v>4.1839455305265116E-2</v>
+        <v>-0.67438312436291015</v>
       </c>
       <c r="U448">
         <v>0</v>
@@ -62103,7 +62122,7 @@
     </row>
     <row r="449" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A449" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B449" s="6">
         <v>0</v>
@@ -62112,7 +62131,7 @@
         <v>0</v>
       </c>
       <c r="D449" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E449" s="6">
         <v>0</v>
@@ -62154,10 +62173,10 @@
         <v>0</v>
       </c>
       <c r="S449">
-        <v>0.23981562534263409</v>
+        <v>0.85843549641073569</v>
       </c>
       <c r="T449">
-        <v>0.91738208776535912</v>
+        <v>4.1839455305265116E-2</v>
       </c>
       <c r="U449">
         <v>0</v>
@@ -62165,7 +62184,7 @@
     </row>
     <row r="450" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A450" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B450" s="6">
         <v>0</v>
@@ -62216,10 +62235,10 @@
         <v>0</v>
       </c>
       <c r="S450">
-        <v>-0.97867806009453584</v>
+        <v>0.23981562534263409</v>
       </c>
       <c r="T450">
-        <v>0.23273645549738398</v>
+        <v>0.91738208776535912</v>
       </c>
       <c r="U450">
         <v>0</v>
@@ -62227,7 +62246,7 @@
     </row>
     <row r="451" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A451" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B451" s="6">
         <v>0</v>
@@ -62242,7 +62261,7 @@
         <v>0</v>
       </c>
       <c r="F451" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G451" s="6">
         <v>0</v>
@@ -62278,10 +62297,10 @@
         <v>0</v>
       </c>
       <c r="S451">
-        <v>-2.0472032919394385</v>
+        <v>-0.97867806009453584</v>
       </c>
       <c r="T451">
-        <v>-0.52367496631650046</v>
+        <v>0.23273645549738398</v>
       </c>
       <c r="U451">
         <v>0</v>
@@ -62289,7 +62308,7 @@
     </row>
     <row r="452" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A452" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B452" s="6">
         <v>0</v>
@@ -62301,10 +62320,10 @@
         <v>0</v>
       </c>
       <c r="E452" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F452" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G452" s="6">
         <v>0</v>
@@ -62340,10 +62359,10 @@
         <v>0</v>
       </c>
       <c r="S452">
-        <v>1.1878304926937509</v>
+        <v>-2.0472032919394385</v>
       </c>
       <c r="T452">
-        <v>-0.62271175588985539</v>
+        <v>-0.52367496631650046</v>
       </c>
       <c r="U452">
         <v>0</v>
@@ -62351,13 +62370,13 @@
     </row>
     <row r="453" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A453" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B453" s="6">
         <v>0</v>
       </c>
       <c r="C453" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D453" s="6">
         <v>0</v>
@@ -62366,7 +62385,7 @@
         <v>1</v>
       </c>
       <c r="F453" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G453" s="6">
         <v>0</v>
@@ -62402,10 +62421,10 @@
         <v>0</v>
       </c>
       <c r="S453">
-        <v>1.7555682098644763</v>
+        <v>1.1878304926937509</v>
       </c>
       <c r="T453">
-        <v>-0.48492143996170944</v>
+        <v>-0.62271175588985539</v>
       </c>
       <c r="U453">
         <v>0</v>
@@ -62413,7 +62432,7 @@
     </row>
     <row r="454" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A454" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B454" s="6">
         <v>0</v>
@@ -62422,13 +62441,13 @@
         <v>1</v>
       </c>
       <c r="D454" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E454" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F454" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G454" s="6">
         <v>0</v>
@@ -62464,10 +62483,10 @@
         <v>0</v>
       </c>
       <c r="S454">
-        <v>1.4261732135814611</v>
+        <v>1.7555682098644763</v>
       </c>
       <c r="T454">
-        <v>-0.86815075613686532</v>
+        <v>-0.48492143996170944</v>
       </c>
       <c r="U454">
         <v>0</v>
@@ -62475,16 +62494,16 @@
     </row>
     <row r="455" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A455" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B455" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C455" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D455" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E455" s="6">
         <v>0</v>
@@ -62526,10 +62545,10 @@
         <v>0</v>
       </c>
       <c r="S455">
-        <v>0.25856168204166746</v>
+        <v>1.4261732135814611</v>
       </c>
       <c r="T455">
-        <v>-0.90977491407349276</v>
+        <v>-0.86815075613686532</v>
       </c>
       <c r="U455">
         <v>0</v>
@@ -62537,10 +62556,10 @@
     </row>
     <row r="456" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A456" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B456" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C456" s="6">
         <v>0</v>
@@ -62555,7 +62574,7 @@
         <v>0</v>
       </c>
       <c r="G456" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I456" s="9">
         <v>2016</v>
@@ -62588,10 +62607,10 @@
         <v>0</v>
       </c>
       <c r="S456">
-        <v>-5.4765265642176215E-2</v>
+        <v>0.25856168204166746</v>
       </c>
       <c r="T456">
-        <v>-0.30837759767877249</v>
+        <v>-0.90977491407349276</v>
       </c>
       <c r="U456">
         <v>0</v>
@@ -62599,7 +62618,7 @@
     </row>
     <row r="457" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A457" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B457" s="6">
         <v>0</v>
@@ -62617,7 +62636,7 @@
         <v>0</v>
       </c>
       <c r="G457" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I457" s="9">
         <v>2016</v>
@@ -62650,10 +62669,10 @@
         <v>0</v>
       </c>
       <c r="S457">
-        <v>-1.2384448457811412</v>
+        <v>-5.4765265642176215E-2</v>
       </c>
       <c r="T457">
-        <v>-0.94996375621920204</v>
+        <v>-0.30837759767877249</v>
       </c>
       <c r="U457">
         <v>0</v>
@@ -62661,7 +62680,7 @@
     </row>
     <row r="458" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A458" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B458" s="6">
         <v>0</v>
@@ -62676,7 +62695,7 @@
         <v>0</v>
       </c>
       <c r="F458" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G458" s="6">
         <v>0</v>
@@ -62712,10 +62731,10 @@
         <v>0</v>
       </c>
       <c r="S458">
-        <v>0.36032598983642011</v>
+        <v>-1.2384448457811412</v>
       </c>
       <c r="T458">
-        <v>-7.2985807968189834E-2</v>
+        <v>-0.94996375621920204</v>
       </c>
       <c r="U458">
         <v>0</v>
@@ -62723,7 +62742,7 @@
     </row>
     <row r="459" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A459" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B459" s="6">
         <v>0</v>
@@ -62774,10 +62793,10 @@
         <v>0</v>
       </c>
       <c r="S459">
-        <v>0.85843549641073569</v>
+        <v>0.36032598983642011</v>
       </c>
       <c r="T459">
-        <v>6.7675139541792481E-2</v>
+        <v>-7.2985807968189834E-2</v>
       </c>
       <c r="U459">
         <v>0</v>
@@ -62785,7 +62804,7 @@
     </row>
     <row r="460" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A460" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B460" s="6">
         <v>0</v>
@@ -62800,7 +62819,7 @@
         <v>0</v>
       </c>
       <c r="F460" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G460" s="6">
         <v>0</v>
@@ -62836,10 +62855,10 @@
         <v>0</v>
       </c>
       <c r="S460">
-        <v>1.581497683373452</v>
+        <v>0.85843549641073569</v>
       </c>
       <c r="T460">
-        <v>-0.51075712419823682</v>
+        <v>6.7675139541792481E-2</v>
       </c>
       <c r="U460">
         <v>0</v>
@@ -62847,7 +62866,7 @@
     </row>
     <row r="461" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A461" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B461" s="6">
         <v>0</v>
@@ -62862,7 +62881,7 @@
         <v>0</v>
       </c>
       <c r="F461" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G461" s="6">
         <v>0</v>
@@ -62898,10 +62917,10 @@
         <v>0</v>
       </c>
       <c r="S461">
-        <v>0.75131517241625922</v>
+        <v>1.581497683373452</v>
       </c>
       <c r="T461">
-        <v>-0.57104038741680063</v>
+        <v>-0.51075712419823682</v>
       </c>
       <c r="U461">
         <v>0</v>
@@ -62909,7 +62928,7 @@
     </row>
     <row r="462" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A462" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B462" s="6">
         <v>0</v>
@@ -62924,7 +62943,7 @@
         <v>0</v>
       </c>
       <c r="F462" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G462" s="6">
         <v>0</v>
@@ -62960,10 +62979,10 @@
         <v>0</v>
       </c>
       <c r="S462">
-        <v>0.62812679982261133</v>
+        <v>0.75131517241625922</v>
       </c>
       <c r="T462">
-        <v>1.1125850353302325</v>
+        <v>-0.57104038741680063</v>
       </c>
       <c r="U462">
         <v>0</v>
@@ -62971,7 +62990,7 @@
     </row>
     <row r="463" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A463" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B463" s="6">
         <v>0</v>
@@ -63022,10 +63041,10 @@
         <v>0</v>
       </c>
       <c r="S463">
-        <v>-0.33863412422753886</v>
+        <v>0.62812679982261133</v>
       </c>
       <c r="T463">
-        <v>5.4757297423528799E-2</v>
+        <v>1.1125850353302325</v>
       </c>
       <c r="U463">
         <v>0</v>
@@ -63033,7 +63052,7 @@
     </row>
     <row r="464" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A464" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B464" s="6">
         <v>0</v>
@@ -63084,10 +63103,10 @@
         <v>0</v>
       </c>
       <c r="S464">
-        <v>-1.5571278096647088</v>
+        <v>-0.33863412422753886</v>
       </c>
       <c r="T464">
-        <v>-0.50788649261640051</v>
+        <v>5.4757297423528799E-2</v>
       </c>
       <c r="U464">
         <v>0</v>
@@ -63095,7 +63114,7 @@
     </row>
     <row r="465" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A465" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B465" s="6">
         <v>0</v>
@@ -63104,7 +63123,7 @@
         <v>0</v>
       </c>
       <c r="D465" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E465" s="6">
         <v>0</v>
@@ -63146,10 +63165,10 @@
         <v>0</v>
       </c>
       <c r="S465">
-        <v>0.68972098611943522</v>
+        <v>-1.5571278096647088</v>
       </c>
       <c r="T465">
-        <v>0.53271745579928498</v>
+        <v>-0.50788649261640051</v>
       </c>
       <c r="U465">
         <v>0</v>
@@ -63157,7 +63176,7 @@
     </row>
     <row r="466" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A466" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B466" s="6">
         <v>0</v>
@@ -63166,7 +63185,7 @@
         <v>0</v>
       </c>
       <c r="D466" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E466" s="6">
         <v>0</v>
@@ -63175,7 +63194,7 @@
         <v>0</v>
       </c>
       <c r="G466" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I466" s="9">
         <v>2016</v>
@@ -63208,10 +63227,10 @@
         <v>0</v>
       </c>
       <c r="S466">
-        <v>0.85575748831087384</v>
+        <v>0.68972098611943522</v>
       </c>
       <c r="T466">
-        <v>-0.81217344029105609</v>
+        <v>0.53271745579928498</v>
       </c>
       <c r="U466">
         <v>0</v>
@@ -63219,7 +63238,7 @@
     </row>
     <row r="467" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A467" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B467" s="6">
         <v>0</v>
@@ -63237,7 +63256,7 @@
         <v>0</v>
       </c>
       <c r="G467" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I467" s="9">
         <v>2016</v>
@@ -63270,10 +63289,10 @@
         <v>0</v>
       </c>
       <c r="S467">
-        <v>1.0164379743025884</v>
+        <v>0.85575748831087384</v>
       </c>
       <c r="T467">
-        <v>-1.7008492122380547E-2</v>
+        <v>-0.81217344029105609</v>
       </c>
       <c r="U467">
         <v>0</v>
@@ -63281,7 +63300,7 @@
     </row>
     <row r="468" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A468" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B468" s="6">
         <v>0</v>
@@ -63332,10 +63351,10 @@
         <v>0</v>
       </c>
       <c r="S468">
-        <v>0.56921062162564928</v>
+        <v>1.0164379743025884</v>
       </c>
       <c r="T468">
-        <v>2.0024808256995086</v>
+        <v>-1.7008492122380547E-2</v>
       </c>
       <c r="U468">
         <v>0</v>
@@ -63343,7 +63362,7 @@
     </row>
     <row r="469" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A469" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B469" s="6">
         <v>0</v>
@@ -63394,10 +63413,10 @@
         <v>0</v>
       </c>
       <c r="S469">
-        <v>-9.225737904024299E-2</v>
+        <v>0.56921062162564928</v>
       </c>
       <c r="T469">
-        <v>0.96761814044749561</v>
+        <v>2.0024808256995086</v>
       </c>
       <c r="U469">
         <v>0</v>
@@ -63405,7 +63424,7 @@
     </row>
     <row r="470" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A470" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B470" s="6">
         <v>0</v>
@@ -63417,10 +63436,10 @@
         <v>0</v>
       </c>
       <c r="E470" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F470" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G470" s="6">
         <v>0</v>
@@ -63456,10 +63475,10 @@
         <v>0</v>
       </c>
       <c r="S470">
-        <v>-1.5437377691653993</v>
+        <v>-9.225737904024299E-2</v>
       </c>
       <c r="T470">
-        <v>-0.93848122989185656</v>
+        <v>0.96761814044749561</v>
       </c>
       <c r="U470">
         <v>0</v>
@@ -63467,7 +63486,7 @@
     </row>
     <row r="471" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A471" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B471" s="6">
         <v>0</v>
@@ -63485,7 +63504,7 @@
         <v>1</v>
       </c>
       <c r="G471" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I471" s="9">
         <v>2016</v>
@@ -63518,10 +63537,10 @@
         <v>0</v>
       </c>
       <c r="S471">
-        <v>0.62009277552302555</v>
+        <v>-1.5437377691653993</v>
       </c>
       <c r="T471">
-        <v>0.49826987681724855</v>
+        <v>-0.93848122989185656</v>
       </c>
       <c r="U471">
         <v>0</v>
@@ -63529,10 +63548,10 @@
     </row>
     <row r="472" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A472" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B472" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C472" s="6">
         <v>0</v>
@@ -63541,13 +63560,13 @@
         <v>0</v>
       </c>
       <c r="E472" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F472" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G472" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I472" s="9">
         <v>2016</v>
@@ -63580,10 +63599,10 @@
         <v>0</v>
       </c>
       <c r="S472">
-        <v>0.3737160303357297</v>
+        <v>0.62009277552302555</v>
       </c>
       <c r="T472">
-        <v>1.4183072987958063</v>
+        <v>0.49826987681724855</v>
       </c>
       <c r="U472">
         <v>0</v>
@@ -63591,10 +63610,10 @@
     </row>
     <row r="473" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A473" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B473" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C473" s="6">
         <v>0</v>
@@ -63642,10 +63661,10 @@
         <v>0</v>
       </c>
       <c r="S473">
-        <v>-0.30917603512905784</v>
+        <v>0.3737160303357297</v>
       </c>
       <c r="T473">
-        <v>2.7818573001680842</v>
+        <v>1.4183072987958063</v>
       </c>
       <c r="U473">
         <v>0</v>
@@ -63653,7 +63672,7 @@
     </row>
     <row r="474" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A474" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B474" s="6">
         <v>0</v>
@@ -63668,7 +63687,7 @@
         <v>0</v>
       </c>
       <c r="F474" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G474" s="6">
         <v>0</v>
@@ -63704,10 +63723,10 @@
         <v>0</v>
       </c>
       <c r="S474">
-        <v>-1.1607826108851458</v>
+        <v>-0.30917603512905784</v>
       </c>
       <c r="T474">
-        <v>-0.49353333470721861</v>
+        <v>2.7818573001680842</v>
       </c>
       <c r="U474">
         <v>0</v>
@@ -63715,10 +63734,10 @@
     </row>
     <row r="475" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A475" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B475" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C475" s="6">
         <v>0</v>
@@ -63766,10 +63785,10 @@
         <v>0</v>
       </c>
       <c r="S475">
-        <v>0.57724464592523494</v>
+        <v>-1.1607826108851458</v>
       </c>
       <c r="T475">
-        <v>1.8874402650574124E-2</v>
+        <v>-0.49353333470721861</v>
       </c>
       <c r="U475">
         <v>0</v>
@@ -63777,10 +63796,10 @@
     </row>
     <row r="476" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A476" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B476" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C476" s="6">
         <v>0</v>
@@ -63792,7 +63811,7 @@
         <v>0</v>
       </c>
       <c r="F476" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G476" s="6">
         <v>0</v>
@@ -63828,10 +63847,10 @@
         <v>0</v>
       </c>
       <c r="S476">
-        <v>0.32818989263807719</v>
+        <v>0.57724464592523494</v>
       </c>
       <c r="T476">
-        <v>2.0096574046540994</v>
+        <v>1.8874402650574124E-2</v>
       </c>
       <c r="U476">
         <v>0</v>
@@ -63839,7 +63858,7 @@
     </row>
     <row r="477" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A477" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B477" s="6">
         <v>0</v>
@@ -63890,10 +63909,10 @@
         <v>0</v>
       </c>
       <c r="S477">
-        <v>-8.957937094038107E-2</v>
+        <v>0.32818989263807719</v>
       </c>
       <c r="T477">
-        <v>3.3459364059989314</v>
+        <v>2.0096574046540994</v>
       </c>
       <c r="U477">
         <v>0</v>
@@ -63901,7 +63920,7 @@
     </row>
     <row r="478" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A478" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B478" s="6">
         <v>0</v>
@@ -63913,7 +63932,7 @@
         <v>0</v>
       </c>
       <c r="E478" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F478" s="6">
         <v>0</v>
@@ -63952,10 +63971,10 @@
         <v>0</v>
       </c>
       <c r="S478">
-        <v>-1.1099004569877695</v>
+        <v>-8.957937094038107E-2</v>
       </c>
       <c r="T478">
-        <v>-0.29258912397867243</v>
+        <v>3.3459364059989314</v>
       </c>
       <c r="U478">
         <v>0</v>
@@ -63963,25 +63982,25 @@
     </row>
     <row r="479" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A479" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B479" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C479" s="6">
         <v>0</v>
       </c>
       <c r="D479" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E479" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F479" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G479" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I479" s="9">
         <v>2016</v>
@@ -64014,10 +64033,10 @@
         <v>0</v>
       </c>
       <c r="S479">
-        <v>1.5573956104746947</v>
+        <v>-1.1099004569877695</v>
       </c>
       <c r="T479">
-        <v>0.3389498240253298</v>
+        <v>-0.29258912397867243</v>
       </c>
       <c r="U479">
         <v>0</v>
@@ -64025,19 +64044,19 @@
     </row>
     <row r="480" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A480" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B480" s="6">
         <v>1</v>
       </c>
       <c r="C480" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D480" s="6">
         <v>1</v>
       </c>
       <c r="E480" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F480" s="6">
         <v>1</v>
@@ -64076,10 +64095,10 @@
         <v>0</v>
       </c>
       <c r="S480">
-        <v>1.6430918696702759</v>
+        <v>1.5573956104746947</v>
       </c>
       <c r="T480">
-        <v>2.3096384049560004</v>
+        <v>0.3389498240253298</v>
       </c>
       <c r="U480">
         <v>0</v>
@@ -64087,28 +64106,28 @@
     </row>
     <row r="481" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A481" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B481" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C481" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D481" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E481" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F481" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G481" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="B481" s="6">
+        <v>1</v>
+      </c>
+      <c r="C481" s="6">
+        <v>1</v>
+      </c>
+      <c r="D481" s="6">
+        <v>1</v>
+      </c>
+      <c r="E481" s="6">
+        <v>1</v>
+      </c>
+      <c r="F481" s="6">
+        <v>1</v>
+      </c>
+      <c r="G481" s="6">
+        <v>1</v>
       </c>
       <c r="I481" s="9">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="J481">
         <v>0</v>
@@ -64132,16 +64151,16 @@
         <v>0</v>
       </c>
       <c r="Q481">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R481">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S481">
-        <v>0.9253856989072835</v>
+        <v>1.6430918696702759</v>
       </c>
       <c r="T481">
-        <v>2.6153606684215744</v>
+        <v>2.3096384049560004</v>
       </c>
       <c r="U481">
         <v>0</v>
@@ -64149,25 +64168,25 @@
     </row>
     <row r="482" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A482" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B482" s="6">
-        <v>0</v>
-      </c>
-      <c r="C482" s="6">
-        <v>0</v>
-      </c>
-      <c r="D482" s="6">
-        <v>0</v>
-      </c>
-      <c r="E482" s="6">
-        <v>0</v>
-      </c>
-      <c r="F482" s="6">
-        <v>0</v>
-      </c>
-      <c r="G482" s="6">
-        <v>0</v>
+        <v>78</v>
+      </c>
+      <c r="B482" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C482" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D482" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E482" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F482" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G482" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="I482" s="9">
         <v>2017</v>
@@ -64200,10 +64219,10 @@
         <v>1</v>
       </c>
       <c r="S482">
-        <v>0.4995824110292395</v>
+        <v>0.9253856989072835</v>
       </c>
       <c r="T482">
-        <v>-0.25527091341479957</v>
+        <v>2.6153606684215744</v>
       </c>
       <c r="U482">
         <v>0</v>
@@ -64211,7 +64230,7 @@
     </row>
     <row r="483" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A483" s="10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B483" s="6">
         <v>0</v>
@@ -64223,7 +64242,7 @@
         <v>0</v>
       </c>
       <c r="E483" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F483" s="6">
         <v>0</v>
@@ -64262,10 +64281,10 @@
         <v>1</v>
       </c>
       <c r="S483">
-        <v>-1.1152564731874932</v>
+        <v>0.4995824110292395</v>
       </c>
       <c r="T483">
-        <v>-0.4705682820525276</v>
+        <v>-0.25527091341479957</v>
       </c>
       <c r="U483">
         <v>0</v>
@@ -64273,22 +64292,22 @@
     </row>
     <row r="484" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A484" s="10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B484" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C484" s="6">
         <v>0</v>
       </c>
       <c r="D484" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E484" s="6">
         <v>1</v>
       </c>
       <c r="F484" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G484" s="6">
         <v>0</v>
@@ -64324,10 +64343,10 @@
         <v>1</v>
       </c>
       <c r="S484">
-        <v>-2.0123891866412338</v>
+        <v>-1.1152564731874932</v>
       </c>
       <c r="T484">
-        <v>-0.48922738733446403</v>
+        <v>-0.4705682820525276</v>
       </c>
       <c r="U484">
         <v>0</v>
@@ -64335,22 +64354,22 @@
     </row>
     <row r="485" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A485" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B485" s="6">
         <v>1</v>
       </c>
       <c r="C485" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D485" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E485" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F485" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G485" s="6">
         <v>0</v>
@@ -64386,10 +64405,10 @@
         <v>1</v>
       </c>
       <c r="S485">
-        <v>0.87182553691004527</v>
+        <v>-2.0123891866412338</v>
       </c>
       <c r="T485">
-        <v>-0.58395822953506438</v>
+        <v>-0.48922738733446403</v>
       </c>
       <c r="U485">
         <v>0</v>
@@ -64397,16 +64416,16 @@
     </row>
     <row r="486" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A486" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B486" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C486" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D486" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E486" s="6">
         <v>0</v>
@@ -64448,10 +64467,10 @@
         <v>1</v>
       </c>
       <c r="S486">
-        <v>0.75399318051612119</v>
+        <v>0.87182553691004527</v>
       </c>
       <c r="T486">
-        <v>-0.79351433500911961</v>
+        <v>-0.58395822953506438</v>
       </c>
       <c r="U486">
         <v>0</v>
@@ -64459,7 +64478,7 @@
     </row>
     <row r="487" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A487" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B487" s="6">
         <v>0</v>
@@ -64468,7 +64487,7 @@
         <v>0</v>
       </c>
       <c r="D487" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E487" s="6">
         <v>0</v>
@@ -64510,10 +64529,10 @@
         <v>1</v>
       </c>
       <c r="S487">
-        <v>0.5370745244273063</v>
+        <v>0.75399318051612119</v>
       </c>
       <c r="T487">
-        <v>-0.45047386097967296</v>
+        <v>-0.79351433500911961</v>
       </c>
       <c r="U487">
         <v>0</v>
@@ -64521,7 +64540,7 @@
     </row>
     <row r="488" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A488" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B488" s="6">
         <v>0</v>
@@ -64572,10 +64591,10 @@
         <v>1</v>
       </c>
       <c r="S488">
-        <v>-0.456466480621463</v>
+        <v>0.5370745244273063</v>
       </c>
       <c r="T488">
-        <v>-0.47487422942528218</v>
+        <v>-0.45047386097967296</v>
       </c>
       <c r="U488">
         <v>0</v>
@@ -64583,13 +64602,13 @@
     </row>
     <row r="489" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A489" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B489" s="6">
         <v>0</v>
       </c>
       <c r="C489" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D489" s="6">
         <v>0</v>
@@ -64598,7 +64617,7 @@
         <v>0</v>
       </c>
       <c r="F489" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G489" s="6">
         <v>0</v>
@@ -64634,10 +64653,10 @@
         <v>1</v>
       </c>
       <c r="S489">
-        <v>-1.340209153575894</v>
+        <v>-0.456466480621463</v>
       </c>
       <c r="T489">
-        <v>-0.36435491352458177</v>
+        <v>-0.47487422942528218</v>
       </c>
       <c r="U489">
         <v>0</v>
@@ -64645,22 +64664,22 @@
     </row>
     <row r="490" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A490" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B490" s="6">
         <v>0</v>
       </c>
       <c r="C490" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D490" s="6">
         <v>0</v>
       </c>
       <c r="E490" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F490" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G490" s="6">
         <v>0</v>
@@ -64696,10 +64715,10 @@
         <v>1</v>
       </c>
       <c r="S490">
-        <v>0.60938074312357793</v>
+        <v>-1.340209153575894</v>
       </c>
       <c r="T490">
-        <v>-0.61122922956250991</v>
+        <v>-0.36435491352458177</v>
       </c>
       <c r="U490">
         <v>0</v>
@@ -64707,10 +64726,10 @@
     </row>
     <row r="491" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A491" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B491" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C491" s="6">
         <v>0</v>
@@ -64719,7 +64738,7 @@
         <v>0</v>
       </c>
       <c r="E491" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F491" s="6">
         <v>0</v>
@@ -64758,10 +64777,10 @@
         <v>1</v>
       </c>
       <c r="S491">
-        <v>0.58795667832468257</v>
+        <v>0.60938074312357793</v>
       </c>
       <c r="T491">
-        <v>-0.57821696637139164</v>
+        <v>-0.61122922956250991</v>
       </c>
       <c r="U491">
         <v>0</v>
@@ -64769,10 +64788,10 @@
     </row>
     <row r="492" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A492" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B492" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C492" s="6">
         <v>0</v>
@@ -64820,10 +64839,10 @@
         <v>1</v>
       </c>
       <c r="S492">
-        <v>0.3763940384355916</v>
+        <v>0.58795667832468257</v>
       </c>
       <c r="T492">
-        <v>-0.63562959800811913</v>
+        <v>-0.57821696637139164</v>
       </c>
       <c r="U492">
         <v>0</v>
@@ -64831,16 +64850,16 @@
     </row>
     <row r="493" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A493" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B493" s="6">
         <v>0</v>
       </c>
       <c r="C493" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D493" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E493" s="6">
         <v>0</v>
@@ -64882,10 +64901,10 @@
         <v>1</v>
       </c>
       <c r="S493">
-        <v>-0.70552123390862076</v>
+        <v>0.3763940384355916</v>
       </c>
       <c r="T493">
-        <v>0.20259482388810204</v>
+        <v>-0.63562959800811913</v>
       </c>
       <c r="U493">
         <v>0</v>
@@ -64893,25 +64912,25 @@
     </row>
     <row r="494" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A494" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B494" s="6">
         <v>0</v>
       </c>
       <c r="C494" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D494" s="6">
         <v>1</v>
       </c>
       <c r="E494" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F494" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G494" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I494" s="9">
         <v>2017</v>
@@ -64944,10 +64963,10 @@
         <v>1</v>
       </c>
       <c r="S494">
-        <v>0.41388615183365834</v>
+        <v>-0.70552123390862076</v>
       </c>
       <c r="T494">
-        <v>-5.0020755313498845E-2</v>
+        <v>0.20259482388810204</v>
       </c>
       <c r="U494">
         <v>0</v>
@@ -64955,7 +64974,7 @@
     </row>
     <row r="495" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A495" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B495" s="6">
         <v>0</v>
@@ -64964,7 +64983,7 @@
         <v>0</v>
       </c>
       <c r="D495" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E495" s="6">
         <v>1</v>
@@ -64973,7 +64992,7 @@
         <v>1</v>
       </c>
       <c r="G495" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I495" s="9">
         <v>2017</v>
@@ -65006,10 +65025,10 @@
         <v>1</v>
       </c>
       <c r="S495">
-        <v>0.2237475767434626</v>
+        <v>0.41388615183365834</v>
       </c>
       <c r="T495">
-        <v>-0.21077612389633577</v>
+        <v>-5.0020755313498845E-2</v>
       </c>
       <c r="U495">
         <v>0</v>
@@ -65017,7 +65036,7 @@
     </row>
     <row r="496" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A496" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B496" s="6">
         <v>0</v>
@@ -65029,10 +65048,10 @@
         <v>0</v>
       </c>
       <c r="E496" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F496" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G496" s="6">
         <v>0</v>
@@ -65068,10 +65087,10 @@
         <v>1</v>
       </c>
       <c r="S496">
-        <v>-0.61446895851331584</v>
+        <v>0.2237475767434626</v>
       </c>
       <c r="T496">
-        <v>-0.40884970304304558</v>
+        <v>-0.21077612389633577</v>
       </c>
       <c r="U496">
         <v>0</v>
@@ -65079,10 +65098,10 @@
     </row>
     <row r="497" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A497" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B497" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C497" s="6">
         <v>0</v>
@@ -65097,7 +65116,7 @@
         <v>0</v>
       </c>
       <c r="G497" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I497" s="9">
         <v>2017</v>
@@ -65130,10 +65149,10 @@
         <v>1</v>
       </c>
       <c r="S497">
-        <v>-1.1018664326881837</v>
+        <v>-0.61446895851331584</v>
       </c>
       <c r="T497">
-        <v>-0.93561059831002014</v>
+        <v>-0.40884970304304558</v>
       </c>
       <c r="U497">
         <v>0</v>
@@ -65141,10 +65160,10 @@
     </row>
     <row r="498" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A498" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B498" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C498" s="6">
         <v>0</v>
@@ -65159,7 +65178,7 @@
         <v>0</v>
       </c>
       <c r="G498" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I498" s="9">
         <v>2017</v>
@@ -65192,10 +65211,10 @@
         <v>1</v>
       </c>
       <c r="S498">
-        <v>-1.2196987890821078</v>
+        <v>-1.1018664326881837</v>
       </c>
       <c r="T498">
-        <v>-0.49066270312538224</v>
+        <v>-0.93561059831002014</v>
       </c>
       <c r="U498">
         <v>0</v>
@@ -65203,7 +65222,7 @@
     </row>
     <row r="499" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A499" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B499" s="6">
         <v>0</v>
@@ -65254,10 +65273,10 @@
         <v>1</v>
       </c>
       <c r="S499">
-        <v>-0.50467062641897742</v>
+        <v>-1.2196987890821078</v>
       </c>
       <c r="T499">
-        <v>-0.46626233467977302</v>
+        <v>-0.49066270312538224</v>
       </c>
       <c r="U499">
         <v>0</v>
@@ -65265,7 +65284,7 @@
     </row>
     <row r="500" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A500" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B500" s="6">
         <v>0</v>
@@ -65316,10 +65335,10 @@
         <v>1</v>
       </c>
       <c r="S500">
-        <v>-1.5705178501640182</v>
+        <v>-0.50467062641897742</v>
       </c>
       <c r="T500">
-        <v>-0.62701770326260997</v>
+        <v>-0.46626233467977302</v>
       </c>
       <c r="U500">
         <v>0</v>
@@ -65327,7 +65346,7 @@
     </row>
     <row r="501" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A501" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B501" s="6">
         <v>0</v>
@@ -65378,10 +65397,10 @@
         <v>1</v>
       </c>
       <c r="S501">
-        <v>-1.6535361012597376</v>
+        <v>-1.5705178501640182</v>
       </c>
       <c r="T501">
-        <v>-0.86240949297319258</v>
+        <v>-0.62701770326260997</v>
       </c>
       <c r="U501">
         <v>0</v>
@@ -65389,10 +65408,10 @@
     </row>
     <row r="502" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A502" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B502" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C502" s="6">
         <v>0</v>
@@ -65404,7 +65423,7 @@
         <v>0</v>
       </c>
       <c r="F502" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G502" s="6">
         <v>0</v>
@@ -65440,10 +65459,10 @@
         <v>1</v>
       </c>
       <c r="S502">
-        <v>-0.68409716910972551</v>
+        <v>-1.6535361012597376</v>
       </c>
       <c r="T502">
-        <v>-0.88250391404604722</v>
+        <v>-0.86240949297319258</v>
       </c>
       <c r="U502">
         <v>0</v>
@@ -65451,10 +65470,10 @@
     </row>
     <row r="503" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A503" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B503" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C503" s="6">
         <v>0</v>
@@ -65466,7 +65485,7 @@
         <v>0</v>
       </c>
       <c r="F503" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G503" s="6">
         <v>0</v>
@@ -65502,10 +65521,10 @@
         <v>1</v>
       </c>
       <c r="S503">
-        <v>-0.68141916100986355</v>
+        <v>-0.68409716910972551</v>
       </c>
       <c r="T503">
-        <v>-0.61266454535342807</v>
+        <v>-0.88250391404604722</v>
       </c>
       <c r="U503">
         <v>0</v>
@@ -65513,7 +65532,7 @@
     </row>
     <row r="504" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A504" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B504" s="6">
         <v>0</v>
@@ -65564,10 +65583,10 @@
         <v>1</v>
       </c>
       <c r="S504">
-        <v>-9.4935387140104896E-2</v>
+        <v>-0.68141916100986355</v>
       </c>
       <c r="T504">
-        <v>3.0356928977919619E-2</v>
+        <v>-0.61266454535342807</v>
       </c>
       <c r="U504">
         <v>0</v>
@@ -65575,7 +65594,7 @@
     </row>
     <row r="505" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A505" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B505" s="6">
         <v>0</v>
@@ -65626,10 +65645,10 @@
         <v>1</v>
       </c>
       <c r="S505">
-        <v>-1.3455651697756177</v>
+        <v>-9.4935387140104896E-2</v>
       </c>
       <c r="T505">
-        <v>-5.4326702686253406E-2</v>
+        <v>3.0356928977919619E-2</v>
       </c>
       <c r="U505">
         <v>0</v>
@@ -65637,13 +65656,13 @@
     </row>
     <row r="506" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A506" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B506" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C506" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D506" s="6">
         <v>0</v>
@@ -65655,7 +65674,7 @@
         <v>0</v>
       </c>
       <c r="G506" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I506" s="9">
         <v>2017</v>
@@ -65688,10 +65707,10 @@
         <v>1</v>
       </c>
       <c r="S506">
-        <v>0.95484378800576453</v>
+        <v>-1.3455651697756177</v>
       </c>
       <c r="T506">
-        <v>-0.63275896642628271</v>
+        <v>-5.4326702686253406E-2</v>
       </c>
       <c r="U506">
         <v>0</v>
@@ -65699,13 +65718,13 @@
     </row>
     <row r="507" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A507" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B507" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C507" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D507" s="6">
         <v>0</v>
@@ -65717,7 +65736,7 @@
         <v>0</v>
       </c>
       <c r="G507" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I507" s="9">
         <v>2017</v>
@@ -65750,10 +65769,10 @@
         <v>1</v>
       </c>
       <c r="S507">
-        <v>0.72989110761736398</v>
+        <v>0.95484378800576453</v>
       </c>
       <c r="T507">
-        <v>-0.67438312436291015</v>
+        <v>-0.63275896642628271</v>
       </c>
       <c r="U507">
         <v>0</v>
@@ -65761,7 +65780,7 @@
     </row>
     <row r="508" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A508" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B508" s="6">
         <v>0</v>
@@ -65770,7 +65789,7 @@
         <v>0</v>
       </c>
       <c r="D508" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E508" s="6">
         <v>0</v>
@@ -65779,7 +65798,7 @@
         <v>0</v>
       </c>
       <c r="G508" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I508" s="9">
         <v>2017</v>
@@ -65812,10 +65831,10 @@
         <v>1</v>
       </c>
       <c r="S508">
-        <v>0.85843549641073569</v>
+        <v>0.72989110761736398</v>
       </c>
       <c r="T508">
-        <v>4.1839455305265116E-2</v>
+        <v>-0.67438312436291015</v>
       </c>
       <c r="U508">
         <v>0</v>
@@ -65823,7 +65842,7 @@
     </row>
     <row r="509" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A509" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B509" s="6">
         <v>0</v>
@@ -65832,7 +65851,7 @@
         <v>0</v>
       </c>
       <c r="D509" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E509" s="6">
         <v>0</v>
@@ -65841,7 +65860,7 @@
         <v>0</v>
       </c>
       <c r="G509" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I509" s="9">
         <v>2017</v>
@@ -65874,10 +65893,10 @@
         <v>1</v>
       </c>
       <c r="S509">
-        <v>0.23981562534263409</v>
+        <v>0.85843549641073569</v>
       </c>
       <c r="T509">
-        <v>0.91738208776535912</v>
+        <v>4.1839455305265116E-2</v>
       </c>
       <c r="U509">
         <v>0</v>
@@ -65885,7 +65904,7 @@
     </row>
     <row r="510" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A510" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B510" s="6">
         <v>0</v>
@@ -65936,10 +65955,10 @@
         <v>1</v>
       </c>
       <c r="S510">
-        <v>-0.97867806009453584</v>
+        <v>0.23981562534263409</v>
       </c>
       <c r="T510">
-        <v>0.23273645549738398</v>
+        <v>0.91738208776535912</v>
       </c>
       <c r="U510">
         <v>0</v>
@@ -65947,7 +65966,7 @@
     </row>
     <row r="511" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A511" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B511" s="6">
         <v>0</v>
@@ -65998,10 +66017,10 @@
         <v>1</v>
       </c>
       <c r="S511">
-        <v>-2.0472032919394385</v>
+        <v>-0.97867806009453584</v>
       </c>
       <c r="T511">
-        <v>-0.52367496631650046</v>
+        <v>0.23273645549738398</v>
       </c>
       <c r="U511">
         <v>0</v>
@@ -66009,7 +66028,7 @@
     </row>
     <row r="512" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A512" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B512" s="6">
         <v>0</v>
@@ -66021,10 +66040,10 @@
         <v>0</v>
       </c>
       <c r="E512" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F512" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G512" s="6">
         <v>0</v>
@@ -66060,10 +66079,10 @@
         <v>1</v>
       </c>
       <c r="S512">
-        <v>1.1878304926937509</v>
+        <v>-2.0472032919394385</v>
       </c>
       <c r="T512">
-        <v>-0.62271175588985539</v>
+        <v>-0.52367496631650046</v>
       </c>
       <c r="U512">
         <v>0</v>
@@ -66071,13 +66090,13 @@
     </row>
     <row r="513" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A513" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B513" s="6">
         <v>0</v>
       </c>
       <c r="C513" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D513" s="6">
         <v>0</v>
@@ -66086,10 +66105,10 @@
         <v>1</v>
       </c>
       <c r="F513" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G513" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I513" s="9">
         <v>2017</v>
@@ -66122,10 +66141,10 @@
         <v>1</v>
       </c>
       <c r="S513">
-        <v>1.7555682098644763</v>
+        <v>1.1878304926937509</v>
       </c>
       <c r="T513">
-        <v>-0.48492143996170944</v>
+        <v>-0.62271175588985539</v>
       </c>
       <c r="U513">
         <v>0</v>
@@ -66133,25 +66152,25 @@
     </row>
     <row r="514" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A514" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B514" s="6">
         <v>0</v>
       </c>
       <c r="C514" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D514" s="6">
         <v>0</v>
       </c>
       <c r="E514" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F514" s="6">
         <v>0</v>
       </c>
       <c r="G514" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I514" s="9">
         <v>2017</v>
@@ -66184,10 +66203,10 @@
         <v>1</v>
       </c>
       <c r="S514">
-        <v>1.4261732135814611</v>
+        <v>1.7555682098644763</v>
       </c>
       <c r="T514">
-        <v>-0.86815075613686532</v>
+        <v>-0.48492143996170944</v>
       </c>
       <c r="U514">
         <v>0</v>
@@ -66195,7 +66214,7 @@
     </row>
     <row r="515" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A515" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B515" s="6">
         <v>0</v>
@@ -66246,10 +66265,10 @@
         <v>1</v>
       </c>
       <c r="S515">
-        <v>0.25856168204166746</v>
+        <v>1.4261732135814611</v>
       </c>
       <c r="T515">
-        <v>-0.90977491407349276</v>
+        <v>-0.86815075613686532</v>
       </c>
       <c r="U515">
         <v>0</v>
@@ -66257,7 +66276,7 @@
     </row>
     <row r="516" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A516" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B516" s="6">
         <v>0</v>
@@ -66308,10 +66327,10 @@
         <v>1</v>
       </c>
       <c r="S516">
-        <v>-5.4765265642176215E-2</v>
+        <v>0.25856168204166746</v>
       </c>
       <c r="T516">
-        <v>-0.30837759767877249</v>
+        <v>-0.90977491407349276</v>
       </c>
       <c r="U516">
         <v>0</v>
@@ -66319,7 +66338,7 @@
     </row>
     <row r="517" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A517" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B517" s="6">
         <v>0</v>
@@ -66370,10 +66389,10 @@
         <v>1</v>
       </c>
       <c r="S517">
-        <v>-1.2384448457811412</v>
+        <v>-5.4765265642176215E-2</v>
       </c>
       <c r="T517">
-        <v>-0.94996375621920204</v>
+        <v>-0.30837759767877249</v>
       </c>
       <c r="U517">
         <v>0</v>
@@ -66381,7 +66400,7 @@
     </row>
     <row r="518" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A518" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B518" s="6">
         <v>0</v>
@@ -66432,10 +66451,10 @@
         <v>1</v>
       </c>
       <c r="S518">
-        <v>0.36032598983642011</v>
+        <v>-1.2384448457811412</v>
       </c>
       <c r="T518">
-        <v>-7.2985807968189834E-2</v>
+        <v>-0.94996375621920204</v>
       </c>
       <c r="U518">
         <v>0</v>
@@ -66443,7 +66462,7 @@
     </row>
     <row r="519" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A519" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B519" s="6">
         <v>0</v>
@@ -66452,7 +66471,7 @@
         <v>0</v>
       </c>
       <c r="D519" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E519" s="6">
         <v>0</v>
@@ -66494,10 +66513,10 @@
         <v>1</v>
       </c>
       <c r="S519">
-        <v>0.85843549641073569</v>
+        <v>0.36032598983642011</v>
       </c>
       <c r="T519">
-        <v>6.7675139541792481E-2</v>
+        <v>-7.2985807968189834E-2</v>
       </c>
       <c r="U519">
         <v>0</v>
@@ -66505,7 +66524,7 @@
     </row>
     <row r="520" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A520" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B520" s="6">
         <v>0</v>
@@ -66514,13 +66533,13 @@
         <v>0</v>
       </c>
       <c r="D520" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E520" s="6">
         <v>0</v>
       </c>
       <c r="F520" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G520" s="6">
         <v>0</v>
@@ -66556,10 +66575,10 @@
         <v>1</v>
       </c>
       <c r="S520">
-        <v>1.581497683373452</v>
+        <v>0.85843549641073569</v>
       </c>
       <c r="T520">
-        <v>-0.51075712419823682</v>
+        <v>6.7675139541792481E-2</v>
       </c>
       <c r="U520">
         <v>0</v>
@@ -66567,13 +66586,13 @@
     </row>
     <row r="521" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A521" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B521" s="6">
         <v>0</v>
       </c>
       <c r="C521" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D521" s="6">
         <v>0</v>
@@ -66582,10 +66601,10 @@
         <v>0</v>
       </c>
       <c r="F521" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G521" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I521" s="9">
         <v>2017</v>
@@ -66618,10 +66637,10 @@
         <v>1</v>
       </c>
       <c r="S521">
-        <v>0.75131517241625922</v>
+        <v>1.581497683373452</v>
       </c>
       <c r="T521">
-        <v>-0.57104038741680063</v>
+        <v>-0.51075712419823682</v>
       </c>
       <c r="U521">
         <v>0</v>
@@ -66629,13 +66648,13 @@
     </row>
     <row r="522" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A522" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B522" s="6">
         <v>0</v>
       </c>
       <c r="C522" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D522" s="6">
         <v>0</v>
@@ -66647,7 +66666,7 @@
         <v>0</v>
       </c>
       <c r="G522" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I522" s="9">
         <v>2017</v>
@@ -66680,10 +66699,10 @@
         <v>1</v>
       </c>
       <c r="S522">
-        <v>0.62812679982261133</v>
+        <v>0.75131517241625922</v>
       </c>
       <c r="T522">
-        <v>1.1125850353302325</v>
+        <v>-0.57104038741680063</v>
       </c>
       <c r="U522">
         <v>0</v>
@@ -66691,7 +66710,7 @@
     </row>
     <row r="523" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A523" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B523" s="6">
         <v>0</v>
@@ -66742,10 +66761,10 @@
         <v>1</v>
       </c>
       <c r="S523">
-        <v>-0.33863412422753886</v>
+        <v>0.62812679982261133</v>
       </c>
       <c r="T523">
-        <v>5.4757297423528799E-2</v>
+        <v>1.1125850353302325</v>
       </c>
       <c r="U523">
         <v>0</v>
@@ -66753,7 +66772,7 @@
     </row>
     <row r="524" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A524" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B524" s="6">
         <v>0</v>
@@ -66804,10 +66823,10 @@
         <v>1</v>
       </c>
       <c r="S524">
-        <v>-1.5571278096647088</v>
+        <v>-0.33863412422753886</v>
       </c>
       <c r="T524">
-        <v>-0.50788649261640051</v>
+        <v>5.4757297423528799E-2</v>
       </c>
       <c r="U524">
         <v>0</v>
@@ -66815,13 +66834,13 @@
     </row>
     <row r="525" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A525" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B525" s="6">
         <v>0</v>
       </c>
       <c r="C525" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D525" s="6">
         <v>0</v>
@@ -66866,10 +66885,10 @@
         <v>1</v>
       </c>
       <c r="S525">
-        <v>0.68972098611943522</v>
+        <v>-1.5571278096647088</v>
       </c>
       <c r="T525">
-        <v>0.53271745579928498</v>
+        <v>-0.50788649261640051</v>
       </c>
       <c r="U525">
         <v>0</v>
@@ -66877,13 +66896,13 @@
     </row>
     <row r="526" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A526" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B526" s="6">
         <v>0</v>
       </c>
       <c r="C526" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D526" s="6">
         <v>0</v>
@@ -66928,10 +66947,10 @@
         <v>1</v>
       </c>
       <c r="S526">
-        <v>0.85575748831087384</v>
+        <v>0.68972098611943522</v>
       </c>
       <c r="T526">
-        <v>-0.81217344029105609</v>
+        <v>0.53271745579928498</v>
       </c>
       <c r="U526">
         <v>0</v>
@@ -66939,22 +66958,22 @@
     </row>
     <row r="527" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A527" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B527" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C527" s="6">
         <v>0</v>
       </c>
       <c r="D527" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E527" s="6">
         <v>0</v>
       </c>
       <c r="F527" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G527" s="6">
         <v>0</v>
@@ -66990,10 +67009,10 @@
         <v>1</v>
       </c>
       <c r="S527">
-        <v>1.0164379743025884</v>
+        <v>0.85575748831087384</v>
       </c>
       <c r="T527">
-        <v>-1.7008492122380547E-2</v>
+        <v>-0.81217344029105609</v>
       </c>
       <c r="U527">
         <v>0</v>
@@ -67001,22 +67020,22 @@
     </row>
     <row r="528" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A528" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B528" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C528" s="6">
         <v>0</v>
       </c>
       <c r="D528" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E528" s="6">
         <v>0</v>
       </c>
       <c r="F528" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G528" s="6">
         <v>0</v>
@@ -67052,10 +67071,10 @@
         <v>1</v>
       </c>
       <c r="S528">
-        <v>0.56921062162564928</v>
+        <v>1.0164379743025884</v>
       </c>
       <c r="T528">
-        <v>2.0024808256995086</v>
+        <v>-1.7008492122380547E-2</v>
       </c>
       <c r="U528">
         <v>0</v>
@@ -67063,7 +67082,7 @@
     </row>
     <row r="529" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A529" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B529" s="6">
         <v>0</v>
@@ -67114,10 +67133,10 @@
         <v>1</v>
       </c>
       <c r="S529">
-        <v>-9.225737904024299E-2</v>
+        <v>0.56921062162564928</v>
       </c>
       <c r="T529">
-        <v>0.96761814044749561</v>
+        <v>2.0024808256995086</v>
       </c>
       <c r="U529">
         <v>0</v>
@@ -67125,7 +67144,7 @@
     </row>
     <row r="530" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A530" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B530" s="6">
         <v>0</v>
@@ -67176,10 +67195,10 @@
         <v>1</v>
       </c>
       <c r="S530">
-        <v>-1.5437377691653993</v>
+        <v>-9.225737904024299E-2</v>
       </c>
       <c r="T530">
-        <v>-0.93848122989185656</v>
+        <v>0.96761814044749561</v>
       </c>
       <c r="U530">
         <v>0</v>
@@ -67187,22 +67206,22 @@
     </row>
     <row r="531" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A531" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B531" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C531" s="6">
         <v>0</v>
       </c>
       <c r="D531" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E531" s="6">
         <v>0</v>
       </c>
       <c r="F531" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G531" s="6">
         <v>0</v>
@@ -67238,10 +67257,10 @@
         <v>1</v>
       </c>
       <c r="S531">
-        <v>0.62009277552302555</v>
+        <v>-1.5437377691653993</v>
       </c>
       <c r="T531">
-        <v>0.49826987681724855</v>
+        <v>-0.93848122989185656</v>
       </c>
       <c r="U531">
         <v>0</v>
@@ -67249,22 +67268,22 @@
     </row>
     <row r="532" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A532" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B532" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C532" s="6">
         <v>0</v>
       </c>
       <c r="D532" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E532" s="6">
         <v>0</v>
       </c>
       <c r="F532" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G532" s="6">
         <v>0</v>
@@ -67300,10 +67319,10 @@
         <v>1</v>
       </c>
       <c r="S532">
-        <v>0.3737160303357297</v>
+        <v>0.62009277552302555</v>
       </c>
       <c r="T532">
-        <v>1.4183072987958063</v>
+        <v>0.49826987681724855</v>
       </c>
       <c r="U532">
         <v>0</v>
@@ -67311,7 +67330,7 @@
     </row>
     <row r="533" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A533" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B533" s="6">
         <v>0</v>
@@ -67362,10 +67381,10 @@
         <v>1</v>
       </c>
       <c r="S533">
-        <v>-0.30917603512905784</v>
+        <v>0.3737160303357297</v>
       </c>
       <c r="T533">
-        <v>2.7818573001680842</v>
+        <v>1.4183072987958063</v>
       </c>
       <c r="U533">
         <v>0</v>
@@ -67373,7 +67392,7 @@
     </row>
     <row r="534" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A534" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B534" s="6">
         <v>0</v>
@@ -67424,10 +67443,10 @@
         <v>1</v>
       </c>
       <c r="S534">
-        <v>-1.1607826108851458</v>
+        <v>-0.30917603512905784</v>
       </c>
       <c r="T534">
-        <v>-0.49353333470721861</v>
+        <v>2.7818573001680842</v>
       </c>
       <c r="U534">
         <v>0</v>
@@ -67435,7 +67454,7 @@
     </row>
     <row r="535" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A535" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B535" s="6">
         <v>0</v>
@@ -67486,10 +67505,10 @@
         <v>1</v>
       </c>
       <c r="S535">
-        <v>0.57724464592523494</v>
+        <v>-1.1607826108851458</v>
       </c>
       <c r="T535">
-        <v>1.8874402650574124E-2</v>
+        <v>-0.49353333470721861</v>
       </c>
       <c r="U535">
         <v>0</v>
@@ -67497,7 +67516,7 @@
     </row>
     <row r="536" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A536" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B536" s="6">
         <v>0</v>
@@ -67548,10 +67567,10 @@
         <v>1</v>
       </c>
       <c r="S536">
-        <v>0.32818989263807719</v>
+        <v>0.57724464592523494</v>
       </c>
       <c r="T536">
-        <v>2.0096574046540994</v>
+        <v>1.8874402650574124E-2</v>
       </c>
       <c r="U536">
         <v>0</v>
@@ -67559,25 +67578,25 @@
     </row>
     <row r="537" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A537" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B537" s="6">
         <v>0</v>
       </c>
       <c r="C537" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D537" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E537" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F537" s="6">
         <v>0</v>
       </c>
       <c r="G537" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I537" s="9">
         <v>2017</v>
@@ -67610,10 +67629,10 @@
         <v>1</v>
       </c>
       <c r="S537">
-        <v>-8.957937094038107E-2</v>
+        <v>0.32818989263807719</v>
       </c>
       <c r="T537">
-        <v>3.3459364059989314</v>
+        <v>2.0096574046540994</v>
       </c>
       <c r="U537">
         <v>0</v>
@@ -67621,25 +67640,25 @@
     </row>
     <row r="538" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A538" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B538" s="6">
         <v>0</v>
       </c>
       <c r="C538" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D538" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E538" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F538" s="6">
         <v>0</v>
       </c>
       <c r="G538" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I538" s="9">
         <v>2017</v>
@@ -67672,10 +67691,10 @@
         <v>1</v>
       </c>
       <c r="S538">
-        <v>-1.1099004569877695</v>
+        <v>-8.957937094038107E-2</v>
       </c>
       <c r="T538">
-        <v>-0.29258912397867243</v>
+        <v>3.3459364059989314</v>
       </c>
       <c r="U538">
         <v>0</v>
@@ -67683,25 +67702,25 @@
     </row>
     <row r="539" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A539" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B539" s="6">
         <v>0</v>
       </c>
       <c r="C539" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D539" s="6">
         <v>0</v>
       </c>
       <c r="E539" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F539" s="6">
         <v>0</v>
       </c>
       <c r="G539" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I539" s="9">
         <v>2017</v>
@@ -67734,10 +67753,10 @@
         <v>1</v>
       </c>
       <c r="S539">
-        <v>1.5573956104746947</v>
+        <v>-1.1099004569877695</v>
       </c>
       <c r="T539">
-        <v>0.3389498240253298</v>
+        <v>-0.29258912397867243</v>
       </c>
       <c r="U539">
         <v>0</v>
@@ -67745,25 +67764,25 @@
     </row>
     <row r="540" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A540" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B540" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C540" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D540" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E540" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F540" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G540" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I540" s="9">
         <v>2017</v>
@@ -67796,12 +67815,74 @@
         <v>1</v>
       </c>
       <c r="S540">
+        <v>1.5573956104746947</v>
+      </c>
+      <c r="T540">
+        <v>0.3389498240253298</v>
+      </c>
+      <c r="U540">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="541" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A541" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B541" s="6">
+        <v>1</v>
+      </c>
+      <c r="C541" s="6">
+        <v>0</v>
+      </c>
+      <c r="D541" s="6">
+        <v>1</v>
+      </c>
+      <c r="E541" s="6">
+        <v>0</v>
+      </c>
+      <c r="F541" s="6">
+        <v>1</v>
+      </c>
+      <c r="G541" s="6">
+        <v>0</v>
+      </c>
+      <c r="I541" s="9">
+        <v>2017</v>
+      </c>
+      <c r="J541">
+        <v>0</v>
+      </c>
+      <c r="K541">
+        <v>0</v>
+      </c>
+      <c r="L541">
+        <v>0</v>
+      </c>
+      <c r="M541">
+        <v>0</v>
+      </c>
+      <c r="N541">
+        <v>0</v>
+      </c>
+      <c r="O541">
+        <v>0</v>
+      </c>
+      <c r="P541">
+        <v>0</v>
+      </c>
+      <c r="Q541">
+        <v>0</v>
+      </c>
+      <c r="R541">
+        <v>1</v>
+      </c>
+      <c r="S541">
         <v>1.6430918696702759</v>
       </c>
-      <c r="T540">
+      <c r="T541">
         <v>2.3096384049560004</v>
       </c>
-      <c r="U540">
+      <c r="U541">
         <v>0</v>
       </c>
     </row>

</xml_diff>